<commit_message>
add some data to dataset
</commit_message>
<xml_diff>
--- a/gridsearch_results.xlsx
+++ b/gridsearch_results.xlsx
@@ -527,16 +527,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>16.67030159632365</v>
+        <v>5.962288459142049</v>
       </c>
       <c r="B2" t="n">
-        <v>0.2062702126005934</v>
+        <v>0.2950884536539055</v>
       </c>
       <c r="C2" t="n">
-        <v>0.01095239321390788</v>
+        <v>0.005705515543619792</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0005685497603330316</v>
+        <v>0.0004467918512696173</v>
       </c>
       <c r="E2" t="n">
         <v>0.1</v>
@@ -595,16 +595,16 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>13.28134576479594</v>
+        <v>5.663124958674113</v>
       </c>
       <c r="B3" t="n">
-        <v>2.2311182666551</v>
+        <v>0.1786572799174025</v>
       </c>
       <c r="C3" t="n">
-        <v>0.01797207196553548</v>
+        <v>0.005200386047363281</v>
       </c>
       <c r="D3" t="n">
-        <v>0.01579280736352864</v>
+        <v>0.0002822886716117706</v>
       </c>
       <c r="E3" t="n">
         <v>0.1</v>

</xml_diff>

<commit_message>
md files for itfrs and owafrs added
</commit_message>
<xml_diff>
--- a/gridsearch_results.xlsx
+++ b/gridsearch_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T3"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,55 +481,60 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
+          <t>param_frsmote__type</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
           <t>param_frsmote__ub_owa_method_name</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>param_frsmote__ub_tnorm_name</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>param_svc__C</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>param_svc__kernel</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>params</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>split0_test_score</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>split1_test_score</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>split2_test_score</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>mean_test_score</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>std_test_score</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>rank_test_score</t>
         </is>
@@ -537,16 +542,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>18.90453163782756</v>
+        <v>31.11437217394511</v>
       </c>
       <c r="B2" t="n">
-        <v>0.3199230419754226</v>
+        <v>0.1423787465209166</v>
       </c>
       <c r="C2" t="n">
-        <v>0.005662043889363606</v>
+        <v>0.008661905924479166</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0004702490165531474</v>
+        <v>0.002622076923139932</v>
       </c>
       <c r="E2" t="n">
         <v>0.1</v>
@@ -573,58 +578,63 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>linear</t>
+          <t>itfrs</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
           <t>minimum</t>
         </is>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>0.1</v>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>rbf</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>{'frsmote__gaussian_similarity_sigma': 0.1, 'frsmote__lb_implicator_name': 'lukasiewicz', 'frsmote__lb_owa_method_name': 'linear', 'frsmote__similarity': 'gaussian', 'frsmote__similarity_tnorm': 'minimum', 'frsmote__ub_owa_method_name': 'linear', 'frsmote__ub_tnorm_name': 'minimum', 'svc__C': 0.1, 'svc__kernel': 'rbf'}</t>
-        </is>
-      </c>
-      <c r="O2" t="n">
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>{'frsmote__gaussian_similarity_sigma': 0.1, 'frsmote__lb_implicator_name': 'lukasiewicz', 'frsmote__lb_owa_method_name': 'linear', 'frsmote__similarity': 'gaussian', 'frsmote__similarity_tnorm': 'minimum', 'frsmote__type': 'itfrs', 'frsmote__ub_owa_method_name': 'linear', 'frsmote__ub_tnorm_name': 'minimum', 'svc__C': 0.1, 'svc__kernel': 'rbf'}</t>
+        </is>
+      </c>
+      <c r="P2" t="n">
         <v>0.6976744186046512</v>
       </c>
-      <c r="P2" t="n">
-        <v>0.6666666666666666</v>
-      </c>
       <c r="Q2" t="n">
-        <v>0.7317073170731707</v>
+        <v>0.6875</v>
       </c>
       <c r="R2" t="n">
-        <v>0.6986828007814961</v>
+        <v>0.75</v>
       </c>
       <c r="S2" t="n">
-        <v>0.02656230634170916</v>
+        <v>0.7117248062015503</v>
       </c>
       <c r="T2" t="n">
-        <v>2</v>
+        <v>0.0273815332382651</v>
+      </c>
+      <c r="U2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>18.90319736798604</v>
+        <v>31.06540067990621</v>
       </c>
       <c r="B3" t="n">
-        <v>0.05454837110348751</v>
+        <v>0.1872362441023085</v>
       </c>
       <c r="C3" t="n">
-        <v>0.005330085754394531</v>
+        <v>0.007661819458007812</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0004701904938510286</v>
+        <v>0.002053224730052947</v>
       </c>
       <c r="E3" t="n">
         <v>0.1</v>
@@ -641,7 +651,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>linear</t>
+          <t>gaussian</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -651,44 +661,215 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>linear</t>
+          <t>owafrs</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
           <t>minimum</t>
         </is>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>0.1</v>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>rbf</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>{'frsmote__gaussian_similarity_sigma': 0.1, 'frsmote__lb_implicator_name': 'lukasiewicz', 'frsmote__lb_owa_method_name': 'linear', 'frsmote__similarity': 'linear', 'frsmote__similarity_tnorm': 'minimum', 'frsmote__ub_owa_method_name': 'linear', 'frsmote__ub_tnorm_name': 'minimum', 'svc__C': 0.1, 'svc__kernel': 'rbf'}</t>
-        </is>
-      </c>
-      <c r="O3" t="n">
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>{'frsmote__gaussian_similarity_sigma': 0.1, 'frsmote__lb_implicator_name': 'lukasiewicz', 'frsmote__lb_owa_method_name': 'linear', 'frsmote__similarity': 'gaussian', 'frsmote__similarity_tnorm': 'minimum', 'frsmote__type': 'owafrs', 'frsmote__ub_owa_method_name': 'linear', 'frsmote__ub_tnorm_name': 'minimum', 'svc__C': 0.1, 'svc__kernel': 'rbf'}</t>
+        </is>
+      </c>
+      <c r="P3" t="n">
         <v>0.6976744186046512</v>
       </c>
-      <c r="P3" t="n">
-        <v>0.6666666666666666</v>
-      </c>
       <c r="Q3" t="n">
+        <v>0.6875</v>
+      </c>
+      <c r="R3" t="n">
         <v>0.75</v>
       </c>
-      <c r="R3" t="n">
-        <v>0.7047803617571059</v>
-      </c>
       <c r="S3" t="n">
-        <v>0.03438974587650173</v>
+        <v>0.7117248062015503</v>
       </c>
       <c r="T3" t="n">
+        <v>0.0273815332382651</v>
+      </c>
+      <c r="U3" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>30.97878360748291</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.1036403696230571</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.006995995839436849</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.002158913127057153</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>lukasiewicz</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>minimum</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>itfrs</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>minimum</t>
+        </is>
+      </c>
+      <c r="M4" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>rbf</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>{'frsmote__gaussian_similarity_sigma': 0.1, 'frsmote__lb_implicator_name': 'lukasiewicz', 'frsmote__lb_owa_method_name': 'linear', 'frsmote__similarity': 'linear', 'frsmote__similarity_tnorm': 'minimum', 'frsmote__type': 'itfrs', 'frsmote__ub_owa_method_name': 'linear', 'frsmote__ub_tnorm_name': 'minimum', 'svc__C': 0.1, 'svc__kernel': 'rbf'}</t>
+        </is>
+      </c>
+      <c r="P4" t="n">
+        <v>0.6521739130434783</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.6875</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.7368421052631579</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0.692172006102212</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.03472315677086865</v>
+      </c>
+      <c r="U4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>30.9464750289917</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.06694761131597743</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.005334854125976562</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.0004688699227739041</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>lukasiewicz</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>minimum</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>owafrs</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>linear</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>minimum</t>
+        </is>
+      </c>
+      <c r="M5" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>rbf</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>{'frsmote__gaussian_similarity_sigma': 0.1, 'frsmote__lb_implicator_name': 'lukasiewicz', 'frsmote__lb_owa_method_name': 'linear', 'frsmote__similarity': 'linear', 'frsmote__similarity_tnorm': 'minimum', 'frsmote__type': 'owafrs', 'frsmote__ub_owa_method_name': 'linear', 'frsmote__ub_tnorm_name': 'minimum', 'svc__C': 0.1, 'svc__kernel': 'rbf'}</t>
+        </is>
+      </c>
+      <c r="P5" t="n">
+        <v>0.6521739130434783</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.6875</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.7368421052631579</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0.692172006102212</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.03472315677086865</v>
+      </c>
+      <c r="U5" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cupy support started to implement-not finished
</commit_message>
<xml_diff>
--- a/gridsearch_results.xlsx
+++ b/gridsearch_results.xlsx
@@ -542,16 +542,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>31.11437217394511</v>
+        <v>7.569942235946655</v>
       </c>
       <c r="B2" t="n">
-        <v>0.1423787465209166</v>
+        <v>0.2483266922241177</v>
       </c>
       <c r="C2" t="n">
-        <v>0.008661905924479166</v>
+        <v>0.008884032567342123</v>
       </c>
       <c r="D2" t="n">
-        <v>0.002622076923139932</v>
+        <v>0.0003953944015714425</v>
       </c>
       <c r="E2" t="n">
         <v>0.1</v>
@@ -625,16 +625,16 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>31.06540067990621</v>
+        <v>8.050627628962198</v>
       </c>
       <c r="B3" t="n">
-        <v>0.1872362441023085</v>
+        <v>0.241196467824371</v>
       </c>
       <c r="C3" t="n">
-        <v>0.007661819458007812</v>
+        <v>0.008636871973673502</v>
       </c>
       <c r="D3" t="n">
-        <v>0.002053224730052947</v>
+        <v>6.781442914425014e-05</v>
       </c>
       <c r="E3" t="n">
         <v>0.1</v>
@@ -708,16 +708,16 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>30.97878360748291</v>
+        <v>7.154925028483073</v>
       </c>
       <c r="B4" t="n">
-        <v>0.1036403696230571</v>
+        <v>0.9695102346140136</v>
       </c>
       <c r="C4" t="n">
-        <v>0.006995995839436849</v>
+        <v>0.005666255950927734</v>
       </c>
       <c r="D4" t="n">
-        <v>0.002158913127057153</v>
+        <v>0.002421370739839173</v>
       </c>
       <c r="E4" t="n">
         <v>0.1</v>
@@ -791,16 +791,16 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>30.9464750289917</v>
+        <v>5.427624861399333</v>
       </c>
       <c r="B5" t="n">
-        <v>0.06694761131597743</v>
+        <v>0.2813850455954224</v>
       </c>
       <c r="C5" t="n">
-        <v>0.005334854125976562</v>
+        <v>0.002858956654866537</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0004688699227739041</v>
+        <v>4.942010690644381e-05</v>
       </c>
       <c r="E5" t="n">
         <v>0.1</v>

</xml_diff>